<commit_message>
Implementação do WebService e alteração nos arquivos de Apresentação do CDI
</commit_message>
<xml_diff>
--- a/docs/Apoio ao Projeto/CheckList/CheckList_Caso_de_Uso.xlsx
+++ b/docs/Apoio ao Projeto/CheckList/CheckList_Caso_de_Uso.xlsx
@@ -1,25 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\EasyLab\docs\Apoio ao Projeto\CheckList\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -92,7 +82,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,21 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -174,6 +152,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -236,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -288,7 +282,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -482,7 +476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,255 +487,255 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50" style="3" customWidth="1"/>
-    <col min="3" max="5" width="4.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="8" width="4.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="1" customWidth="1"/>
+    <col min="3" max="5" width="4.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="8" width="4.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="3">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="3">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="3">
         <v>8</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="3">
         <v>9</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="N472dIjkt6YrjtD2qEj5lAW772MmH/Zz088k7/bcSNYrl84f7bfFu2SKZomGs89NHEduL+k8+yNIFeqqjuXF2g==" saltValue="eIdkQtQGM02qfX7o3wACBg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection password="EEB7" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="10">
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:I4"/>

</xml_diff>